<commit_message>
doing June reporting, also find that we can do Liquidity reporting using Jupyter notebook
</commit_message>
<xml_diff>
--- a/FX.xlsx
+++ b/FX.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steven.zhang\AppData\Local\Programs\Git\git\risk_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECFA049C-B025-46D5-970A-5BFF31EEBE68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{503CCD6D-E847-48F4-A68C-36858B889423}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30780" yWindow="615" windowWidth="21960" windowHeight="14850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
   <si>
     <t>Date</t>
   </si>
@@ -382,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,6 +457,20 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>44012</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>7.7504999999999997</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
finished 2020-09-30 LQA and Asset Allocation reports
</commit_message>
<xml_diff>
--- a/FX.xlsx
+++ b/FX.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steven.zhang\AppData\Local\Programs\Git\git\risk_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{503CCD6D-E847-48F4-A68C-36858B889423}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B9A9770-A63B-4876-B305-E3854CDFF6BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35475" yWindow="1545" windowWidth="20490" windowHeight="12840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t>Date</t>
   </si>
@@ -382,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,6 +471,20 @@
         <v>7.7504999999999997</v>
       </c>
     </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>44104</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>7.75</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
generated DIF 20201030 liquidity and asset allocation reports
</commit_message>
<xml_diff>
--- a/FX.xlsx
+++ b/FX.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steven.zhang\AppData\Local\Programs\Git\git\risk_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B9A9770-A63B-4876-B305-E3854CDFF6BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{106F4847-166E-4BF2-A349-4D0BB4589FD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35475" yWindow="1545" windowWidth="20490" windowHeight="12840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
   <si>
     <t>Date</t>
   </si>
@@ -382,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,6 +485,20 @@
         <v>7.75</v>
       </c>
     </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>44134</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>7.7522000000000002</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
finished DIF 2020-12-31 report
</commit_message>
<xml_diff>
--- a/FX.xlsx
+++ b/FX.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steven.zhang\AppData\Local\Programs\Git\git\risk_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{106F4847-166E-4BF2-A349-4D0BB4589FD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A5DA4D3-E6B1-4AC8-86FA-D76140CF9B6B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34245" yWindow="1815" windowWidth="17970" windowHeight="12135" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="7">
   <si>
     <t>Date</t>
   </si>
@@ -382,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,6 +499,20 @@
         <v>7.7522000000000002</v>
       </c>
     </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>44196</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>7.7530999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
finished 19437 and 60001 2021 Mar reports. But getLqaData() needs to be updated
</commit_message>
<xml_diff>
--- a/FX.xlsx
+++ b/FX.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steven.zhang\AppData\Local\Programs\Git\git\risk_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A5DA4D3-E6B1-4AC8-86FA-D76140CF9B6B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5414A3EB-884B-4A67-A27F-71E4402E3B9C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34245" yWindow="1815" windowWidth="17970" windowHeight="12135" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31215" yWindow="1260" windowWidth="15165" windowHeight="12510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="7">
   <si>
     <t>Date</t>
   </si>
@@ -382,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,6 +513,20 @@
         <v>7.7530999999999999</v>
       </c>
     </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>44286</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>7.7740999999999998</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
generated both 19437 and 60001 June 2021 report
</commit_message>
<xml_diff>
--- a/FX.xlsx
+++ b/FX.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steven.zhang\AppData\Local\Programs\Git\git\risk_report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhangst\git\risk_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5414A3EB-884B-4A67-A27F-71E4402E3B9C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA67E4B-4DCE-4C97-BA4D-F22E294D4D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31215" yWindow="1260" windowWidth="15165" windowHeight="12510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="7">
   <si>
     <t>Date</t>
   </si>
@@ -382,20 +382,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -409,7 +409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>43950</v>
       </c>
@@ -423,7 +423,7 @@
         <v>7.7519999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>43980</v>
       </c>
@@ -437,7 +437,7 @@
         <v>7.7511999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>43980</v>
       </c>
@@ -457,7 +457,7 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>44012</v>
       </c>
@@ -471,7 +471,7 @@
         <v>7.7504999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>44104</v>
       </c>
@@ -485,7 +485,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>44134</v>
       </c>
@@ -499,7 +499,7 @@
         <v>7.7522000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>44196</v>
       </c>
@@ -513,7 +513,7 @@
         <v>7.7530999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>44286</v>
       </c>
@@ -525,6 +525,20 @@
       </c>
       <c r="D9">
         <v>7.7740999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>44377</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>7.7651000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>